<commit_message>
Cambios Plan de Pruebas
</commit_message>
<xml_diff>
--- a/Proyectos/ControlDeGastos/03. Desarrollo/ControlDeGastos-PlanPruebas.xlsx
+++ b/Proyectos/ControlDeGastos/03. Desarrollo/ControlDeGastos-PlanPruebas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t>ID</t>
   </si>
@@ -114,9 +114,6 @@
     <t xml:space="preserve">Validar la funcionalidad del módulo de Subrubro donde se pueda crear, buscar, modificar y eliminar </t>
   </si>
   <si>
-    <t xml:space="preserve">Validar la funcionalidad del módulo de Movimientos donde se pueda crear, buscar, modificar y eliminar </t>
-  </si>
-  <si>
     <t xml:space="preserve">Validar la funcionalidad del módulo de Cuentas donde se pueda crear, buscar, modificar y eliminar </t>
   </si>
   <si>
@@ -163,6 +160,12 @@
   </si>
   <si>
     <t>CU13</t>
+  </si>
+  <si>
+    <t>Validar la funcionalidad del módulo de Movimientos donde se pueda crear, buscar, modificar y eliminar . Además validar que al realizar el traspaso de cuenta en movimiento se refleje en dichos movimientos.</t>
+  </si>
+  <si>
+    <t>No actualiza la lista de subrubro, no actualiza la lista de la cuenta.</t>
   </si>
 </sst>
 </file>
@@ -385,17 +388,17 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -748,7 +751,7 @@
   <dimension ref="B1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -756,7 +759,7 @@
     <col min="1" max="1" width="2.140625" style="5" customWidth="1"/>
     <col min="2" max="2" width="5.42578125" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="24" style="5" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="5" customWidth="1"/>
     <col min="5" max="5" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="11.85546875" style="5" customWidth="1"/>
     <col min="8" max="8" width="33.28515625" style="5" customWidth="1"/>
@@ -770,10 +773,10 @@
     <row r="2" spans="2:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C3" s="8"/>
-      <c r="D3" s="17" t="s">
+      <c r="D3" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="17"/>
+      <c r="E3" s="20"/>
     </row>
     <row r="5" spans="2:11" s="7" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="6" t="s">
@@ -807,18 +810,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B6" s="9">
         <v>1</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C6" s="17" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="11" t="s">
         <v>29</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F6" s="12">
         <v>42492</v>
@@ -839,14 +842,14 @@
       <c r="B7" s="9">
         <v>2</v>
       </c>
-      <c r="C7" s="18" t="s">
+      <c r="C7" s="17" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="11" t="s">
         <v>30</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="12">
         <v>42492</v>
@@ -863,18 +866,18 @@
       </c>
       <c r="K7" s="15"/>
     </row>
-    <row r="8" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:11" ht="115.5" x14ac:dyDescent="0.3">
       <c r="B8" s="9">
         <v>3</v>
       </c>
-      <c r="C8" s="18" t="s">
+      <c r="C8" s="17" t="s">
         <v>16</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" s="12">
         <v>42492</v>
@@ -882,7 +885,9 @@
       <c r="G8" s="12">
         <v>42493</v>
       </c>
-      <c r="H8" s="10"/>
+      <c r="H8" s="11" t="s">
+        <v>48</v>
+      </c>
       <c r="I8" s="10" t="s">
         <v>9</v>
       </c>
@@ -895,14 +900,14 @@
       <c r="B9" s="9">
         <v>4</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="17" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="12">
         <v>42492</v>
@@ -923,14 +928,14 @@
       <c r="B10" s="9">
         <v>5</v>
       </c>
-      <c r="C10" s="19" t="s">
+      <c r="C10" s="18" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F10" s="12">
         <v>42492</v>
@@ -947,18 +952,18 @@
       </c>
       <c r="K10" s="15"/>
     </row>
-    <row r="11" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B11" s="9">
         <v>6</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="C11" s="18" t="s">
         <v>19</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" s="12">
         <v>42492</v>
@@ -975,18 +980,18 @@
       </c>
       <c r="K11" s="15"/>
     </row>
-    <row r="12" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B12" s="9">
         <v>7</v>
       </c>
-      <c r="C12" s="19" t="s">
+      <c r="C12" s="18" t="s">
         <v>20</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F12" s="12">
         <v>42492</v>
@@ -1003,15 +1008,15 @@
       </c>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
       <c r="B13" s="9">
         <v>8</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="19" t="s">
         <v>21</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="10" t="s">
         <v>10</v>
@@ -1035,11 +1040,11 @@
       <c r="B14" s="9">
         <v>9</v>
       </c>
-      <c r="C14" s="19" t="s">
+      <c r="C14" s="18" t="s">
         <v>22</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E14" s="10" t="s">
         <v>10</v>
@@ -1059,15 +1064,15 @@
       </c>
       <c r="K14" s="13"/>
     </row>
-    <row r="15" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" ht="33" x14ac:dyDescent="0.3">
       <c r="B15" s="14">
         <v>10</v>
       </c>
-      <c r="C15" s="18" t="s">
+      <c r="C15" s="17" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>10</v>
@@ -1091,11 +1096,11 @@
       <c r="B16" s="9">
         <v>11</v>
       </c>
-      <c r="C16" s="18" t="s">
+      <c r="C16" s="17" t="s">
         <v>28</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E16" s="10" t="s">
         <v>10</v>
@@ -1119,11 +1124,11 @@
       <c r="B17" s="9">
         <v>12</v>
       </c>
-      <c r="C17" s="18" t="s">
+      <c r="C17" s="17" t="s">
         <v>24</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>10</v>
@@ -1147,11 +1152,11 @@
       <c r="B18" s="9">
         <v>13</v>
       </c>
-      <c r="C18" s="18" t="s">
+      <c r="C18" s="17" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E18" s="10" t="s">
         <v>10</v>
@@ -1175,11 +1180,11 @@
       <c r="B19" s="9">
         <v>14</v>
       </c>
-      <c r="C19" s="19" t="s">
+      <c r="C19" s="18" t="s">
         <v>26</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E19" s="10" t="s">
         <v>10</v>
@@ -1203,11 +1208,11 @@
       <c r="B20" s="9">
         <v>15</v>
       </c>
-      <c r="C20" s="19" t="s">
+      <c r="C20" s="18" t="s">
         <v>27</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>10</v>
@@ -1243,12 +1248,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1301,9 +1303,12 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1311,9 +1316,16 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8A0BA0D-EB78-4A30-8F1E-2355421FFA94}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BD56E88-2DE2-4D0C-B13B-E9AD00E5579C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1334,16 +1346,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BD56E88-2DE2-4D0C-B13B-E9AD00E5579C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8A0BA0D-EB78-4A30-8F1E-2355421FFA94}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
Actualizacion Plan de Pruebas
</commit_message>
<xml_diff>
--- a/Proyectos/ControlDeGastos/03. Desarrollo/ControlDeGastos-PlanPruebas.xlsx
+++ b/Proyectos/ControlDeGastos/03. Desarrollo/ControlDeGastos-PlanPruebas.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="66">
   <si>
     <t>ID</t>
   </si>
@@ -54,9 +54,6 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>En Proceso</t>
-  </si>
-  <si>
     <t>Resultados</t>
   </si>
   <si>
@@ -102,9 +99,6 @@
     <t>Sencilla de utilizar, no tener que dar muchos clicks para generar alguna consulta o registro</t>
   </si>
   <si>
-    <t>Mostrar mensajes cuando crea algún registro para no replicarlo nuevamente</t>
-  </si>
-  <si>
     <t>Interfaz sencilla basada en botones y cajas de texto, para las consultas de movimientos mostrar gráficos que reflejen los gastos e ingresos</t>
   </si>
   <si>
@@ -126,18 +120,12 @@
     <t>Asegurar que  se generen la visualización de la consulta  de gastos e ingresos por Cuenta</t>
   </si>
   <si>
-    <t>Validar la visualización de de la gráfica de gastos e ingresos al realizar la consulta</t>
-  </si>
-  <si>
     <t>Confirmar que la interfaz sea amigable para el usuario.</t>
   </si>
   <si>
     <t>Asegurar que la aplicación sea independiente de la conexión a internet</t>
   </si>
   <si>
-    <t>Validar que se muestre en pantalla el mensaje en caso de información duplicada</t>
-  </si>
-  <si>
     <t>Validar el acceso solo a usuarios registrados</t>
   </si>
   <si>
@@ -162,17 +150,80 @@
     <t>CU13</t>
   </si>
   <si>
-    <t>Validar la funcionalidad del módulo de Movimientos donde se pueda crear, buscar, modificar y eliminar . Además validar que al realizar el traspaso de cuenta en movimiento se refleje en dichos movimientos.</t>
-  </si>
-  <si>
     <t>No actualiza la lista de subrubro, no actualiza la lista de la cuenta.</t>
+  </si>
+  <si>
+    <t>Se pueden realizar traspasos entre cuentas</t>
+  </si>
+  <si>
+    <t>Validar que se realicen los traspasos entre las cuentas del usuario</t>
+  </si>
+  <si>
+    <t>Validar la funcionalidad del módulo de Movimientos donde se pueda crear, buscar, modificar y eliminar .</t>
+  </si>
+  <si>
+    <t>Aprobado</t>
+  </si>
+  <si>
+    <t>Validar la visualización de la gráfica de gastos e ingresos al realizar la consulta</t>
+  </si>
+  <si>
+    <t>Para el módulo de SubRubro, se pueden obtener las opciones de crear, buscar, modificar y eliminar</t>
+  </si>
+  <si>
+    <t>Se obtiene dentro del módulo de Rubro las opciones para crear, buscar, modificar y eliminar.</t>
+  </si>
+  <si>
+    <t>Se obtiene dentro del módulo de Movimientos las opciones para crear, buscar, modificar y eliminar. Se corrigió la correcta visualización de la lista de subrubro y la lista de la cuenta.</t>
+  </si>
+  <si>
+    <t>El tiempo de respuesta se considera apropiado</t>
+  </si>
+  <si>
+    <t>Interfaz amigable para el usuario, manejo de pestañas con las diferentes secciones</t>
+  </si>
+  <si>
+    <t>Aplicación en el equipo del usuario, solo se permite el ingreso a usuarios registrados</t>
+  </si>
+  <si>
+    <t>Se presentan las secciones separadas por pestañas con el título de la sección, facilitando la interacción con el usuario.</t>
+  </si>
+  <si>
+    <t>Los movimientos de traspasos quedan registrados en la cuenta que se realizan</t>
+  </si>
+  <si>
+    <t>Al ingresar nuevo, que el campo de ID se deshabilite, no muestra el saldo correcto ingresado</t>
+  </si>
+  <si>
+    <t>Aplicación de escritorio, directo en el equipo del usuario.</t>
+  </si>
+  <si>
+    <t>Es una aplicación de escritorio, no genera conflictos.</t>
+  </si>
+  <si>
+    <t>El módulo de Cuentas permite la creación de una cuenta, su búsqueda, modificación y eliminación.</t>
+  </si>
+  <si>
+    <t>Dentro de rubros se tiene la opción de mostrar gastos e ingresos según se elija el tipo de movimiento.</t>
+  </si>
+  <si>
+    <t>Para subrubro se puede realizar la consulta para gasto o ingreso, de acuerdo al movimiento elegido.</t>
+  </si>
+  <si>
+    <t>En Cuenta se muestra el movimiento de gasto o ingreso para su consulta.</t>
+  </si>
+  <si>
+    <t>Se tiene la opción de mostrar la gráfica para gastos o ingresos, al realizar una consulta, se determina el periódo del cual se requiere la presentación.</t>
+  </si>
+  <si>
+    <t>La gráfica no se muestra completa si el periodo que se requiere visualizar es de un solo mes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -207,12 +258,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Arial Narrow"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Arial Narrow"/>
       <family val="2"/>
     </font>
@@ -338,9 +383,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -348,9 +393,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -385,17 +427,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -751,486 +793,520 @@
   <dimension ref="B1:K20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A5" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.140625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="5.42578125" style="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.42578125" style="5" customWidth="1"/>
-    <col min="4" max="4" width="28.85546875" style="5" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.85546875" style="5" customWidth="1"/>
-    <col min="8" max="8" width="33.28515625" style="5" customWidth="1"/>
-    <col min="9" max="9" width="22.85546875" style="5" customWidth="1"/>
-    <col min="10" max="10" width="10.140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="54.5703125" style="5" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="5"/>
+    <col min="1" max="1" width="2.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.42578125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.85546875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="33.28515625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="10.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="54.5703125" style="4" customWidth="1"/>
+    <col min="12" max="16384" width="11.42578125" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:11" ht="67.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:11" ht="10.5" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:11" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="8"/>
-      <c r="D3" s="20" t="s">
+      <c r="C3" s="7"/>
+      <c r="D3" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="19"/>
+    </row>
+    <row r="5" spans="2:11" s="6" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="20"/>
-    </row>
-    <row r="5" spans="2:11" s="7" customFormat="1" ht="39" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="D6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" s="11">
+        <v>42492</v>
+      </c>
+      <c r="G6" s="11">
+        <v>42493</v>
+      </c>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K6" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="B7" s="8">
         <v>2</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="C7" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="11">
+        <v>42492</v>
+      </c>
+      <c r="G7" s="11">
+        <v>42493</v>
+      </c>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="B8" s="8">
         <v>3</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="C8" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="11">
+        <v>42492</v>
+      </c>
+      <c r="G8" s="11">
+        <v>42493</v>
+      </c>
+      <c r="H8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="B9" s="8">
         <v>4</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="C9" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="F9" s="11">
+        <v>42492</v>
+      </c>
+      <c r="G9" s="11">
+        <v>42493</v>
+      </c>
+      <c r="H9" s="9"/>
+      <c r="I9" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="B10" s="8">
         <v>5</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="C10" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F10" s="11">
+        <v>42492</v>
+      </c>
+      <c r="G10" s="11">
+        <v>42493</v>
+      </c>
+      <c r="H10" s="9"/>
+      <c r="I10" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K10" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B11" s="8">
         <v>6</v>
       </c>
-      <c r="I5" s="6" t="s">
+      <c r="C11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F11" s="11">
+        <v>42492</v>
+      </c>
+      <c r="G11" s="11">
+        <v>42493</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" s="14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B12" s="8">
         <v>7</v>
       </c>
-      <c r="J5" s="6" t="s">
+      <c r="C12" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="11">
+        <v>42492</v>
+      </c>
+      <c r="G12" s="11">
+        <v>42493</v>
+      </c>
+      <c r="H12" s="9"/>
+      <c r="I12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B13" s="8">
         <v>8</v>
       </c>
-      <c r="K5" s="6" t="s">
+      <c r="C13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="11">
+        <v>42492</v>
+      </c>
+      <c r="G13" s="11">
+        <v>42493</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
+      <c r="B14" s="8">
+        <v>9</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="11">
+        <v>42492</v>
+      </c>
+      <c r="G14" s="11">
+        <v>42493</v>
+      </c>
+      <c r="H14" s="1"/>
+      <c r="I14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="33" x14ac:dyDescent="0.3">
+      <c r="B15" s="13">
+        <v>10</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="11">
+        <v>42492</v>
+      </c>
+      <c r="G15" s="11">
+        <v>42493</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K15" s="12" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="82.5" x14ac:dyDescent="0.3">
+      <c r="B16" s="8">
+        <v>11</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F16" s="11">
+        <v>42492</v>
+      </c>
+      <c r="G16" s="11">
+        <v>42493</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K16" s="14" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="B17" s="8">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B6" s="9">
-        <v>1</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="F6" s="12">
-        <v>42492</v>
-      </c>
-      <c r="G6" s="12">
-        <v>42493</v>
-      </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K6" s="16"/>
-    </row>
-    <row r="7" spans="2:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="B7" s="9">
-        <v>2</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="12">
-        <v>42492</v>
-      </c>
-      <c r="G7" s="12">
-        <v>42493</v>
-      </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="15"/>
-    </row>
-    <row r="8" spans="2:11" ht="115.5" x14ac:dyDescent="0.3">
-      <c r="B8" s="9">
-        <v>3</v>
-      </c>
-      <c r="C8" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="12">
-        <v>42492</v>
-      </c>
-      <c r="G8" s="12">
-        <v>42493</v>
-      </c>
-      <c r="H8" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="I8" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K8" s="15"/>
-    </row>
-    <row r="9" spans="2:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="B9" s="9">
-        <v>4</v>
-      </c>
-      <c r="C9" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F9" s="12">
-        <v>42492</v>
-      </c>
-      <c r="G9" s="12">
-        <v>42493</v>
-      </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K9" s="15"/>
-    </row>
-    <row r="10" spans="2:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="B10" s="9">
-        <v>5</v>
-      </c>
-      <c r="C10" s="18" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F10" s="12">
-        <v>42492</v>
-      </c>
-      <c r="G10" s="12">
-        <v>42493</v>
-      </c>
-      <c r="H10" s="10"/>
-      <c r="I10" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K10" s="15"/>
-    </row>
-    <row r="11" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B11" s="9">
-        <v>6</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F11" s="12">
-        <v>42492</v>
-      </c>
-      <c r="G11" s="12">
-        <v>42493</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K11" s="15"/>
-    </row>
-    <row r="12" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B12" s="9">
-        <v>7</v>
-      </c>
-      <c r="C12" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>34</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F12" s="12">
-        <v>42492</v>
-      </c>
-      <c r="G12" s="12">
-        <v>42493</v>
-      </c>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B13" s="9">
-        <v>8</v>
-      </c>
-      <c r="C13" s="19" t="s">
-        <v>21</v>
-      </c>
-      <c r="D13" s="11" t="s">
+      <c r="C17" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="10" t="s">
         <v>35</v>
-      </c>
-      <c r="E13" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="12">
-        <v>42492</v>
-      </c>
-      <c r="G13" s="12">
-        <v>42493</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K13" s="13"/>
-    </row>
-    <row r="14" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B14" s="9">
-        <v>9</v>
-      </c>
-      <c r="C14" s="18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F14" s="12">
-        <v>42492</v>
-      </c>
-      <c r="G14" s="12">
-        <v>42493</v>
-      </c>
-      <c r="H14" s="1"/>
-      <c r="I14" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K14" s="13"/>
-    </row>
-    <row r="15" spans="2:11" ht="33" x14ac:dyDescent="0.3">
-      <c r="B15" s="14">
-        <v>10</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F15" s="12">
-        <v>42492</v>
-      </c>
-      <c r="G15" s="12">
-        <v>42493</v>
-      </c>
-      <c r="H15" s="1"/>
-      <c r="I15" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K15" s="13"/>
-    </row>
-    <row r="16" spans="2:11" ht="82.5" x14ac:dyDescent="0.3">
-      <c r="B16" s="9">
-        <v>11</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>28</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F16" s="12">
-        <v>42492</v>
-      </c>
-      <c r="G16" s="12">
-        <v>42493</v>
-      </c>
-      <c r="H16" s="2"/>
-      <c r="I16" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="2:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="B17" s="9">
-        <v>12</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>39</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F17" s="12">
+      <c r="F17" s="11">
         <v>42492</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="11">
         <v>42493</v>
       </c>
       <c r="H17" s="1"/>
-      <c r="I17" s="10" t="s">
+      <c r="I17" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K17" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="18" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B18" s="9">
+      <c r="B18" s="8">
         <v>13</v>
       </c>
-      <c r="C18" s="17" t="s">
+      <c r="C18" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="F18" s="11">
+        <v>42492</v>
+      </c>
+      <c r="G18" s="11">
+        <v>42493</v>
+      </c>
+      <c r="H18" s="1"/>
+      <c r="I18" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="K18" s="12" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:11" ht="66" x14ac:dyDescent="0.3">
+      <c r="B19" s="8">
+        <v>14</v>
+      </c>
+      <c r="C19" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D18" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="D19" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="F18" s="12">
+      <c r="F19" s="11">
         <v>42492</v>
       </c>
-      <c r="G18" s="12">
+      <c r="G19" s="11">
         <v>42493</v>
       </c>
-      <c r="H18" s="1"/>
-      <c r="I18" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="2:11" ht="66" x14ac:dyDescent="0.3">
-      <c r="B19" s="9">
-        <v>14</v>
-      </c>
-      <c r="C19" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="D19" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="E19" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F19" s="12">
-        <v>42492</v>
-      </c>
-      <c r="G19" s="12">
-        <v>42493</v>
-      </c>
       <c r="H19" s="1"/>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K19" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="20" spans="2:11" ht="49.5" x14ac:dyDescent="0.3">
-      <c r="B20" s="9">
+      <c r="B20" s="8">
         <v>15</v>
       </c>
-      <c r="C20" s="18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>38</v>
+      <c r="C20" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="12">
+      <c r="F20" s="11">
         <v>42492</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G20" s="11">
         <v>42493</v>
       </c>
-      <c r="H20" s="1"/>
-      <c r="I20" s="10" t="s">
+      <c r="H20" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="I20" s="9" t="s">
         <v>9</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K20" s="4"/>
+        <v>47</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>